<commit_message>
update master code mabel info
</commit_message>
<xml_diff>
--- a/1_Input_data/MasterCodebook_October.xlsx
+++ b/1_Input_data/MasterCodebook_October.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmunozav/Desktop/Zika_imputation/1_Input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6663F6-777E-704C-A979-4772FB06FB78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE519CD-49C9-4245-B170-56ADE53EBF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="500" windowWidth="24440" windowHeight="14120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1280" yWindow="500" windowWidth="24440" windowHeight="14120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Var count and directions" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,9 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 2" guid="{EB9D8945-92F8-48A6-B1A8-0874D0F705AD}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{9C9CF54D-CE09-4329-9468-764052FC28B8}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 1" guid="{3AF2D2F3-3B31-4BFE-9B21-6EF5937D96DE}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{9C9CF54D-CE09-4329-9468-764052FC28B8}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{EB9D8945-92F8-48A6-B1A8-0874D0F705AD}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -715,7 +715,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12895" uniqueCount="3140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12896" uniqueCount="3140">
   <si>
     <t>Tab</t>
   </si>
@@ -49029,11 +49029,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Y282"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="J11" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B235" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y273" sqref="Y273"/>
+      <selection pane="bottomRight" activeCell="E286" sqref="E286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1"/>
@@ -49500,7 +49500,7 @@
       </c>
       <c r="S10" s="210"/>
     </row>
-    <row r="11" spans="1:25" ht="15" customHeight="1">
+    <row r="11" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A11" s="177" t="s">
         <v>167</v>
       </c>
@@ -49572,7 +49572,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="15" customHeight="1">
+    <row r="12" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A12" s="177" t="s">
         <v>171</v>
       </c>
@@ -49633,7 +49633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="15" customHeight="1">
+    <row r="13" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A13" s="192" t="s">
         <v>174</v>
       </c>
@@ -49692,7 +49692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="15" customHeight="1">
+    <row r="14" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A14" s="177" t="s">
         <v>177</v>
       </c>
@@ -49799,7 +49799,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="15" customHeight="1">
+    <row r="16" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A16" s="177" t="s">
         <v>183</v>
       </c>
@@ -50033,7 +50033,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="15" customHeight="1">
+    <row r="21" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A21" s="192" t="s">
         <v>267</v>
       </c>
@@ -50140,7 +50140,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="15" customHeight="1">
+    <row r="23" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A23" s="192" t="s">
         <v>309</v>
       </c>
@@ -50293,7 +50293,7 @@
         <v>2861</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="15" customHeight="1">
+    <row r="26" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A26" s="177" t="s">
         <v>361</v>
       </c>
@@ -50398,7 +50398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="15" customHeight="1">
+    <row r="28" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A28" s="192" t="s">
         <v>369</v>
       </c>
@@ -50752,7 +50752,7 @@
         <v>2861</v>
       </c>
     </row>
-    <row r="36" spans="1:25" ht="15" customHeight="1">
+    <row r="36" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A36" s="204" t="s">
         <v>395</v>
       </c>
@@ -51723,7 +51723,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="56" spans="1:25" ht="15" customHeight="1">
+    <row r="56" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A56" s="177" t="s">
         <v>482</v>
       </c>
@@ -52275,7 +52275,7 @@
         <v>2862</v>
       </c>
     </row>
-    <row r="67" spans="1:25" ht="15" customHeight="1">
+    <row r="67" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A67" s="203" t="s">
         <v>537</v>
       </c>
@@ -52854,7 +52854,7 @@
         <v>2862</v>
       </c>
     </row>
-    <row r="79" spans="1:25" ht="15" customHeight="1">
+    <row r="79" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A79" s="203" t="s">
         <v>562</v>
       </c>
@@ -52915,7 +52915,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:25" ht="15" customHeight="1">
+    <row r="80" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A80" s="203" t="s">
         <v>565</v>
       </c>
@@ -52974,7 +52974,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:25" ht="15" customHeight="1">
+    <row r="81" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A81" s="192" t="s">
         <v>574</v>
       </c>
@@ -53035,7 +53035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:25" ht="15" customHeight="1">
+    <row r="82" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A82" s="177" t="s">
         <v>702</v>
       </c>
@@ -53392,7 +53392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:25" ht="15" customHeight="1">
+    <row r="89" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A89" s="177" t="s">
         <v>725</v>
       </c>
@@ -53607,7 +53607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:25" ht="15" customHeight="1">
+    <row r="93" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A93" s="177" t="s">
         <v>742</v>
       </c>
@@ -53828,7 +53828,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="97" spans="1:25" ht="15" customHeight="1">
+    <row r="97" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A97" s="177" t="s">
         <v>751</v>
       </c>
@@ -53943,7 +53943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:25" ht="15" customHeight="1">
+    <row r="99" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A99" s="177" t="s">
         <v>755</v>
       </c>
@@ -54058,7 +54058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:25" ht="15" customHeight="1">
+    <row r="101" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A101" s="177" t="s">
         <v>759</v>
       </c>
@@ -54117,7 +54117,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:25" ht="15" customHeight="1">
+    <row r="102" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A102" s="177" t="s">
         <v>761</v>
       </c>
@@ -54178,7 +54178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:25" ht="15" customHeight="1">
+    <row r="103" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A103" s="177" t="s">
         <v>763</v>
       </c>
@@ -54241,7 +54241,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:25" ht="15" customHeight="1">
+    <row r="104" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A104" s="177" t="s">
         <v>768</v>
       </c>
@@ -54302,7 +54302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:25" ht="15" customHeight="1">
+    <row r="105" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A105" s="177" t="s">
         <v>770</v>
       </c>
@@ -54363,7 +54363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:25" ht="15" customHeight="1">
+    <row r="106" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A106" s="177" t="s">
         <v>778</v>
       </c>
@@ -54424,7 +54424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:25" ht="15" customHeight="1">
+    <row r="107" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A107" s="177" t="s">
         <v>780</v>
       </c>
@@ -54727,7 +54727,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="113" spans="1:25" ht="15" customHeight="1">
+    <row r="113" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A113" s="193" t="s">
         <v>811</v>
       </c>
@@ -55047,7 +55047,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="119" spans="1:25" ht="15" customHeight="1">
+    <row r="119" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A119" s="193" t="s">
         <v>839</v>
       </c>
@@ -55167,7 +55167,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="121" spans="1:25" ht="15" customHeight="1">
+    <row r="121" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A121" s="193" t="s">
         <v>846</v>
       </c>
@@ -55423,7 +55423,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="126" spans="1:25" ht="15" customHeight="1">
+    <row r="126" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A126" s="193" t="s">
         <v>860</v>
       </c>
@@ -55479,7 +55479,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="1:25" ht="15" customHeight="1">
+    <row r="127" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A127" s="193" t="s">
         <v>864</v>
       </c>
@@ -55535,7 +55535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:25" ht="15" customHeight="1">
+    <row r="128" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A128" s="193" t="s">
         <v>870</v>
       </c>
@@ -56108,7 +56108,7 @@
         <v>2852</v>
       </c>
     </row>
-    <row r="139" spans="1:25" ht="15" customHeight="1">
+    <row r="139" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A139" s="193" t="s">
         <v>913</v>
       </c>
@@ -56223,7 +56223,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="141" spans="1:25" ht="15" customHeight="1">
+    <row r="141" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A141" s="193" t="s">
         <v>918</v>
       </c>
@@ -57157,7 +57157,7 @@
         <v>2864</v>
       </c>
     </row>
-    <row r="160" spans="1:25" ht="15" customHeight="1">
+    <row r="160" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A160" s="199" t="s">
         <v>1658</v>
       </c>
@@ -57210,7 +57210,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:25" ht="15" customHeight="1">
+    <row r="161" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A161" s="197" t="s">
         <v>1649</v>
       </c>
@@ -57272,7 +57272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:25" ht="15" customHeight="1">
+    <row r="162" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A162" s="197" t="s">
         <v>1640</v>
       </c>
@@ -58679,7 +58679,7 @@
       </c>
       <c r="U191" s="210"/>
     </row>
-    <row r="192" spans="1:25" ht="15" customHeight="1">
+    <row r="192" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A192" s="197" t="s">
         <v>1191</v>
       </c>
@@ -59237,7 +59237,7 @@
       <c r="T202" s="210"/>
       <c r="U202" s="212"/>
     </row>
-    <row r="203" spans="1:24" ht="15" customHeight="1">
+    <row r="203" spans="1:24" ht="15" hidden="1" customHeight="1">
       <c r="A203" s="199" t="s">
         <v>1669</v>
       </c>
@@ -59612,7 +59612,7 @@
       <c r="T211" s="210"/>
       <c r="U211" s="210"/>
     </row>
-    <row r="212" spans="1:25" ht="15" customHeight="1">
+    <row r="212" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A212" s="197" t="s">
         <v>1690</v>
       </c>
@@ -59761,7 +59761,7 @@
       <c r="T214" s="210"/>
       <c r="U214" s="210"/>
     </row>
-    <row r="215" spans="1:25" ht="15" customHeight="1">
+    <row r="215" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A215" s="199" t="s">
         <v>1716</v>
       </c>
@@ -60311,7 +60311,7 @@
       <c r="T225" s="210"/>
       <c r="U225" s="210"/>
     </row>
-    <row r="226" spans="1:25" ht="15" customHeight="1">
+    <row r="226" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A226" s="177" t="s">
         <v>1770</v>
       </c>
@@ -60495,7 +60495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:25" ht="15" customHeight="1">
+    <row r="229" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A229" s="199" t="s">
         <v>1782</v>
       </c>
@@ -60763,7 +60763,7 @@
       </c>
       <c r="U234" s="252"/>
     </row>
-    <row r="235" spans="1:25" ht="15" hidden="1" customHeight="1">
+    <row r="235" spans="1:25" ht="15" customHeight="1">
       <c r="A235" s="239" t="s">
         <v>2605</v>
       </c>
@@ -60799,7 +60799,7 @@
       <c r="O235" s="234"/>
       <c r="P235" s="234"/>
     </row>
-    <row r="236" spans="1:25" ht="15" hidden="1" customHeight="1">
+    <row r="236" spans="1:25" ht="15" customHeight="1">
       <c r="A236" s="236" t="s">
         <v>2870</v>
       </c>
@@ -60807,7 +60807,9 @@
       <c r="C236" s="218" t="s">
         <v>2869</v>
       </c>
-      <c r="D236" s="243"/>
+      <c r="D236" s="243" t="s">
+        <v>121</v>
+      </c>
       <c r="E236" s="243"/>
       <c r="F236" s="252"/>
       <c r="G236" s="177"/>
@@ -60879,7 +60881,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="238" spans="1:25" ht="15" customHeight="1">
+    <row r="238" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A238" s="221" t="s">
         <v>2887</v>
       </c>
@@ -61012,7 +61014,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="241" spans="1:25" ht="15" customHeight="1">
+    <row r="241" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A241" s="221" t="s">
         <v>2888</v>
       </c>
@@ -61179,7 +61181,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="245" spans="1:25" ht="15" customHeight="1">
+    <row r="245" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A245" s="221" t="s">
         <v>2884</v>
       </c>
@@ -61307,7 +61309,7 @@
         <v>2861</v>
       </c>
     </row>
-    <row r="248" spans="1:25" ht="15" customHeight="1">
+    <row r="248" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A248" s="221" t="s">
         <v>2900</v>
       </c>
@@ -61352,7 +61354,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="249" spans="1:25" ht="15" customHeight="1">
+    <row r="249" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A249" s="221" t="s">
         <v>2874</v>
       </c>
@@ -61555,7 +61557,7 @@
         <v>2861</v>
       </c>
     </row>
-    <row r="254" spans="1:25" ht="15" customHeight="1">
+    <row r="254" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A254" s="221" t="s">
         <v>2905</v>
       </c>
@@ -61641,7 +61643,7 @@
         <v>2861</v>
       </c>
     </row>
-    <row r="256" spans="1:25" ht="15" customHeight="1">
+    <row r="256" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A256" s="221" t="s">
         <v>2893</v>
       </c>
@@ -61688,7 +61690,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="257" spans="1:25" ht="15" customHeight="1">
+    <row r="257" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A257" s="221" t="s">
         <v>2907</v>
       </c>
@@ -61735,7 +61737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:25" ht="15" customHeight="1">
+    <row r="258" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A258" s="221" t="s">
         <v>2871</v>
       </c>
@@ -61784,7 +61786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="259" spans="1:25" ht="15" customHeight="1">
+    <row r="259" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A259" s="221" t="s">
         <v>2883</v>
       </c>
@@ -61873,7 +61875,7 @@
         <v>2861</v>
       </c>
     </row>
-    <row r="261" spans="1:25" ht="15" customHeight="1">
+    <row r="261" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A261" s="221" t="s">
         <v>2895</v>
       </c>
@@ -62044,7 +62046,7 @@
         <v>2861</v>
       </c>
     </row>
-    <row r="265" spans="1:25" ht="15" customHeight="1">
+    <row r="265" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A265" s="221" t="s">
         <v>2876</v>
       </c>
@@ -62089,7 +62091,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="266" spans="1:25" ht="15" customHeight="1">
+    <row r="266" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A266" s="221" t="s">
         <v>2877</v>
       </c>
@@ -62134,7 +62136,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="267" spans="1:25" ht="15" customHeight="1">
+    <row r="267" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A267" s="221" t="s">
         <v>2908</v>
       </c>
@@ -62179,7 +62181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="268" spans="1:25" ht="15" customHeight="1">
+    <row r="268" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A268" s="221" t="s">
         <v>2875</v>
       </c>
@@ -62226,7 +62228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:25" ht="15" customHeight="1">
+    <row r="269" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A269" s="221" t="s">
         <v>2879</v>
       </c>
@@ -62268,7 +62270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:25" ht="15" customHeight="1">
+    <row r="270" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A270" s="221" t="s">
         <v>2878</v>
       </c>
@@ -62315,7 +62317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="271" spans="1:25" ht="15" customHeight="1">
+    <row r="271" spans="1:25" ht="15" hidden="1" customHeight="1">
       <c r="A271" s="221" t="s">
         <v>2819</v>
       </c>
@@ -62460,10 +62462,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:X282" xr:uid="{B522DC56-3FF5-3344-845C-95A0430599ED}">
-    <filterColumn colId="6">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
+    <filterColumn colId="0">
+      <filters>
+        <filter val="studycode"/>
+        <filter val="studyimp"/>
+        <filter val="studyname"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X283">
@@ -62751,7 +62755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F0DA957-6899-A948-BF9C-0A6CA3970A65}">
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update harlan message feb6
</commit_message>
<xml_diff>
--- a/1_Input_data/MasterCodebook_October.xlsx
+++ b/1_Input_data/MasterCodebook_October.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmunozav/Desktop/Zika_imputation/1_Input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B910805-2D2A-C24F-BBD1-2584B59F3E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5CFF9B-138A-9843-979A-33011B8E98D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Var count and directions" sheetId="1" r:id="rId1"/>
@@ -21,15 +21,15 @@
     <sheet name="Sheet2" sheetId="10" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'237 key'!$A$1:$AA$289</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'237 key'!$A$1:$AA$290</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ALL!$A$1:$M$992</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">StudyID!$A$1:$R$67</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{3AF2D2F3-3B31-4BFE-9B21-6EF5937D96DE}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{9C9CF54D-CE09-4329-9468-764052FC28B8}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 2" guid="{EB9D8945-92F8-48A6-B1A8-0874D0F705AD}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{9C9CF54D-CE09-4329-9468-764052FC28B8}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{3AF2D2F3-3B31-4BFE-9B21-6EF5937D96DE}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -715,7 +715,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13052" uniqueCount="3167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13056" uniqueCount="3170">
   <si>
     <t>Tab</t>
   </si>
@@ -12013,6 +12013,15 @@
   </si>
   <si>
     <t>Included</t>
+  </si>
+  <si>
+    <t>interaction</t>
+  </si>
+  <si>
+    <t>microcephaly_bin_fet</t>
+  </si>
+  <si>
+    <t>replace fet_micro</t>
   </si>
 </sst>
 </file>
@@ -12715,7 +12724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="269">
+  <cellXfs count="273">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -13437,16 +13446,24 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="58">
+  <dxfs count="162">
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
         </patternFill>
       </fill>
     </dxf>
@@ -13906,6 +13923,838 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -14136,7 +14985,7 @@
   </sheetPr>
   <dimension ref="B1:P997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -15960,7 +16809,7 @@
   </sheetPr>
   <dimension ref="A1:M992"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A280" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I386" sqref="I386"/>
     </sheetView>
@@ -49127,27 +49976,27 @@
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="C2:D218">
-    <cfRule type="containsText" dxfId="57" priority="5" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="161" priority="5" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(C2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C219:D252">
-    <cfRule type="containsText" dxfId="56" priority="4" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="160" priority="4" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(C219))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C253:D321">
-    <cfRule type="containsText" dxfId="55" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="159" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(C253))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C322:D346">
-    <cfRule type="containsText" dxfId="54" priority="2" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="158" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(C322))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C347:C388">
-    <cfRule type="containsText" dxfId="53" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="157" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(C347))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -49172,13 +50021,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B522DC56-3FF5-3344-845C-95A0430599ED}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AA290"/>
+  <dimension ref="A1:AB290"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="M246" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B246" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V294" sqref="V294"/>
+      <selection pane="bottomRight" activeCell="A291" sqref="A291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1"/>
@@ -49196,7 +50045,7 @@
     <col min="20" max="25" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15" customHeight="1">
+    <row r="1" spans="1:28" ht="15" customHeight="1">
       <c r="A1" s="228" t="s">
         <v>3098</v>
       </c>
@@ -49278,8 +50127,11 @@
       <c r="AA1" s="201" t="s">
         <v>3136</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" ht="15" hidden="1" customHeight="1">
+      <c r="AB1" s="201" t="s">
+        <v>3167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A2" s="177" t="s">
         <v>123</v>
       </c>
@@ -49328,7 +50180,7 @@
       <c r="X2" s="83"/>
       <c r="Y2" s="83"/>
     </row>
-    <row r="3" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="3" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A3" s="177" t="s">
         <v>128</v>
       </c>
@@ -49371,7 +50223,7 @@
         <v>2864</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="4" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A4" s="177" t="s">
         <v>132</v>
       </c>
@@ -49414,7 +50266,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="5" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A5" s="177" t="s">
         <v>136</v>
       </c>
@@ -49454,7 +50306,7 @@
         <v>76.291901936959505</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="6" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A6" s="177" t="s">
         <v>138</v>
       </c>
@@ -49494,7 +50346,7 @@
         <v>77.342577371167195</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="7" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A7" s="177" t="s">
         <v>140</v>
       </c>
@@ -49535,7 +50387,7 @@
       </c>
       <c r="T7" s="210"/>
     </row>
-    <row r="8" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="8" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A8" s="177" t="s">
         <v>142</v>
       </c>
@@ -49576,7 +50428,7 @@
       </c>
       <c r="T8" s="210"/>
     </row>
-    <row r="9" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="9" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A9" s="177" t="s">
         <v>144</v>
       </c>
@@ -49617,7 +50469,7 @@
       </c>
       <c r="T9" s="210"/>
     </row>
-    <row r="10" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="10" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A10" s="177" t="s">
         <v>146</v>
       </c>
@@ -49658,7 +50510,7 @@
       </c>
       <c r="T10" s="210"/>
     </row>
-    <row r="11" spans="1:27" ht="15" customHeight="1">
+    <row r="11" spans="1:28" ht="15" customHeight="1">
       <c r="A11" s="177" t="s">
         <v>167</v>
       </c>
@@ -49733,7 +50585,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="12" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A12" s="177" t="s">
         <v>171</v>
       </c>
@@ -49795,7 +50647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="15" customHeight="1">
+    <row r="13" spans="1:28" ht="15" customHeight="1">
       <c r="A13" s="192" t="s">
         <v>174</v>
       </c>
@@ -49857,7 +50709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="15" customHeight="1">
+    <row r="14" spans="1:28" ht="15" customHeight="1">
       <c r="A14" s="177" t="s">
         <v>177</v>
       </c>
@@ -49919,7 +50771,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="15" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A15" s="177" t="s">
         <v>180</v>
       </c>
@@ -49968,7 +50820,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="16" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A16" s="177" t="s">
         <v>183</v>
       </c>
@@ -50033,7 +50885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="17" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A17" s="177" t="s">
         <v>208</v>
       </c>
@@ -50077,7 +50929,7 @@
         <v>2861</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="18" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A18" s="177" t="s">
         <v>247</v>
       </c>
@@ -50121,7 +50973,7 @@
         <v>2861</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="19" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A19" s="177" t="s">
         <v>250</v>
       </c>
@@ -50165,7 +51017,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="20" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A20" s="177" t="s">
         <v>254</v>
       </c>
@@ -50209,7 +51061,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="15" customHeight="1">
+    <row r="21" spans="1:28" ht="15" customHeight="1">
       <c r="A21" s="192" t="s">
         <v>267</v>
       </c>
@@ -50270,8 +51122,11 @@
       <c r="Z21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:26" ht="15" hidden="1" customHeight="1">
+      <c r="AB21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A22" s="202" t="s">
         <v>269</v>
       </c>
@@ -50320,7 +51175,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="15" customHeight="1">
+    <row r="23" spans="1:28" ht="15" customHeight="1">
       <c r="A23" s="192" t="s">
         <v>309</v>
       </c>
@@ -50378,7 +51233,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="24" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A24" s="177" t="s">
         <v>332</v>
       </c>
@@ -50427,7 +51282,7 @@
         <v>2861</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="25" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A25" s="177" t="s">
         <v>347</v>
       </c>
@@ -50476,7 +51331,7 @@
         <v>2861</v>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="15" customHeight="1">
+    <row r="26" spans="1:28" ht="15" customHeight="1">
       <c r="A26" s="177" t="s">
         <v>361</v>
       </c>
@@ -50534,7 +51389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="27" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A27" s="192" t="s">
         <v>365</v>
       </c>
@@ -50583,7 +51438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="28" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A28" s="192" t="s">
         <v>369</v>
       </c>
@@ -50634,7 +51489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="29" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A29" s="203" t="s">
         <v>372</v>
       </c>
@@ -50678,7 +51533,7 @@
         <v>2861</v>
       </c>
     </row>
-    <row r="30" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="30" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A30" s="203" t="s">
         <v>374</v>
       </c>
@@ -50723,7 +51578,7 @@
         <v>2861</v>
       </c>
     </row>
-    <row r="31" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="31" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A31" s="203" t="s">
         <v>376</v>
       </c>
@@ -50768,7 +51623,7 @@
         <v>2861</v>
       </c>
     </row>
-    <row r="32" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="32" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A32" s="203" t="s">
         <v>378</v>
       </c>
@@ -53211,7 +54066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="81" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A81" s="192" t="s">
         <v>574</v>
       </c>
@@ -53276,7 +54131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:27" ht="15" customHeight="1">
+    <row r="82" spans="1:28" ht="15" customHeight="1">
       <c r="A82" s="177" t="s">
         <v>702</v>
       </c>
@@ -53339,8 +54194,11 @@
       <c r="Z82">
         <v>2</v>
       </c>
-    </row>
-    <row r="83" spans="1:27" ht="15" hidden="1" customHeight="1">
+      <c r="AB82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A83" s="177" t="s">
         <v>704</v>
       </c>
@@ -53389,7 +54247,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="84" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="84" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A84" s="177" t="s">
         <v>710</v>
       </c>
@@ -53432,7 +54290,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="85" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="85" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A85" s="177" t="s">
         <v>712</v>
       </c>
@@ -53490,7 +54348,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="86" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="86" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A86" s="177" t="s">
         <v>715</v>
       </c>
@@ -53539,7 +54397,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="87" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="87" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A87" s="177" t="s">
         <v>717</v>
       </c>
@@ -53590,7 +54448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="88" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A88" s="177" t="s">
         <v>721</v>
       </c>
@@ -53641,7 +54499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:27" ht="15" customHeight="1">
+    <row r="89" spans="1:28" ht="15" customHeight="1">
       <c r="A89" s="177" t="s">
         <v>725</v>
       </c>
@@ -53704,8 +54562,11 @@
       <c r="Z89">
         <v>2</v>
       </c>
-    </row>
-    <row r="90" spans="1:27" ht="15" hidden="1" customHeight="1">
+      <c r="AB89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A90" s="177" t="s">
         <v>728</v>
       </c>
@@ -53760,7 +54621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="91" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A91" s="192" t="s">
         <v>733</v>
       </c>
@@ -53805,7 +54666,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="92" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="92" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A92" s="177" t="s">
         <v>739</v>
       </c>
@@ -53862,7 +54723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:27" ht="15" customHeight="1">
+    <row r="93" spans="1:28" ht="15" customHeight="1">
       <c r="A93" s="177" t="s">
         <v>742</v>
       </c>
@@ -53925,8 +54786,11 @@
       <c r="Z93">
         <v>2</v>
       </c>
-    </row>
-    <row r="94" spans="1:27" ht="15" hidden="1" customHeight="1">
+      <c r="AB93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A94" s="177" t="s">
         <v>744</v>
       </c>
@@ -53981,7 +54845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="95" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A95" s="177" t="s">
         <v>746</v>
       </c>
@@ -54038,7 +54902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="96" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A96" s="177" t="s">
         <v>748</v>
       </c>
@@ -54089,7 +54953,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="97" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="97" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A97" s="177" t="s">
         <v>751</v>
       </c>
@@ -54151,7 +55015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="98" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A98" s="177" t="s">
         <v>753</v>
       </c>
@@ -54206,7 +55070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:27" ht="15" customHeight="1">
+    <row r="99" spans="1:28" ht="15" customHeight="1">
       <c r="A99" s="177" t="s">
         <v>755</v>
       </c>
@@ -54269,8 +55133,11 @@
       <c r="Z99">
         <v>2</v>
       </c>
-    </row>
-    <row r="100" spans="1:27" ht="15" hidden="1" customHeight="1">
+      <c r="AB99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A100" s="177" t="s">
         <v>757</v>
       </c>
@@ -54325,7 +55192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:27" ht="15" customHeight="1">
+    <row r="101" spans="1:28" ht="15" customHeight="1">
       <c r="A101" s="177" t="s">
         <v>759</v>
       </c>
@@ -54386,8 +55253,11 @@
       <c r="Z101">
         <v>2</v>
       </c>
-    </row>
-    <row r="102" spans="1:27" ht="15" hidden="1" customHeight="1">
+      <c r="AB101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A102" s="177" t="s">
         <v>761</v>
       </c>
@@ -54452,7 +55322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:27" ht="15" customHeight="1">
+    <row r="103" spans="1:28" ht="15" customHeight="1">
       <c r="A103" s="177" t="s">
         <v>763</v>
       </c>
@@ -54517,8 +55387,11 @@
       <c r="Z103">
         <v>2</v>
       </c>
-    </row>
-    <row r="104" spans="1:27" ht="15" hidden="1" customHeight="1">
+      <c r="AB103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A104" s="177" t="s">
         <v>768</v>
       </c>
@@ -54583,7 +55456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="105" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A105" s="177" t="s">
         <v>770</v>
       </c>
@@ -54645,7 +55518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="106" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A106" s="177" t="s">
         <v>778</v>
       </c>
@@ -54710,7 +55583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="107" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A107" s="177" t="s">
         <v>780</v>
       </c>
@@ -54772,7 +55645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="108" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A108" s="193" t="s">
         <v>791</v>
       </c>
@@ -54821,7 +55694,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="109" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="109" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A109" s="193" t="s">
         <v>798</v>
       </c>
@@ -54870,7 +55743,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="110" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="110" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A110" s="193" t="s">
         <v>802</v>
       </c>
@@ -54925,7 +55798,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="111" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="111" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A111" s="193" t="s">
         <v>805</v>
       </c>
@@ -54971,7 +55844,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="112" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="112" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A112" s="193" t="s">
         <v>809</v>
       </c>
@@ -55902,7 +56775,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="129" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A129" s="193" t="s">
         <v>874</v>
       </c>
@@ -55956,7 +56829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="130" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A130" s="193" t="s">
         <v>879</v>
       </c>
@@ -56004,7 +56877,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="131" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="131" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A131" s="193" t="s">
         <v>881</v>
       </c>
@@ -56058,7 +56931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="132" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A132" s="193" t="s">
         <v>885</v>
       </c>
@@ -56112,7 +56985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="133" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A133" s="193" t="s">
         <v>890</v>
       </c>
@@ -56160,7 +57033,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="134" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="134" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A134" s="193" t="s">
         <v>894</v>
       </c>
@@ -56217,7 +57090,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="135" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="135" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A135" s="193" t="s">
         <v>898</v>
       </c>
@@ -56271,7 +57144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="136" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A136" s="193" t="s">
         <v>901</v>
       </c>
@@ -56325,7 +57198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="137" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A137" s="193" t="s">
         <v>905</v>
       </c>
@@ -56376,7 +57249,7 @@
         <v>2852</v>
       </c>
     </row>
-    <row r="138" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="138" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A138" s="193" t="s">
         <v>909</v>
       </c>
@@ -56427,7 +57300,7 @@
         <v>2852</v>
       </c>
     </row>
-    <row r="139" spans="1:26" ht="15" customHeight="1">
+    <row r="139" spans="1:28" ht="15" customHeight="1">
       <c r="A139" s="193" t="s">
         <v>913</v>
       </c>
@@ -56499,8 +57372,11 @@
       <c r="Z139">
         <v>1</v>
       </c>
-    </row>
-    <row r="140" spans="1:26" ht="15" hidden="1" customHeight="1">
+      <c r="AB139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A140" s="193" t="s">
         <v>916</v>
       </c>
@@ -56546,7 +57422,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="141" spans="1:26" ht="15" customHeight="1">
+    <row r="141" spans="1:28" ht="15" customHeight="1">
       <c r="A141" s="193" t="s">
         <v>918</v>
       </c>
@@ -56616,8 +57492,11 @@
       <c r="Z141">
         <v>2</v>
       </c>
-    </row>
-    <row r="142" spans="1:26" ht="15" hidden="1" customHeight="1">
+      <c r="AB141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A142" s="193" t="s">
         <v>921</v>
       </c>
@@ -56664,7 +57543,7 @@
         <v>2861</v>
       </c>
     </row>
-    <row r="143" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="143" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A143" s="193" t="s">
         <v>924</v>
       </c>
@@ -56713,7 +57592,7 @@
         <v>2861</v>
       </c>
     </row>
-    <row r="144" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="144" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A144" s="193" t="s">
         <v>931</v>
       </c>
@@ -59051,7 +59930,7 @@
       </c>
       <c r="V191" s="210"/>
     </row>
-    <row r="192" spans="1:26" ht="15" customHeight="1">
+    <row r="192" spans="1:26" ht="15" hidden="1" customHeight="1">
       <c r="A192" s="197" t="s">
         <v>1191</v>
       </c>
@@ -59067,7 +59946,7 @@
         <v>120</v>
       </c>
       <c r="G192" s="225" t="s">
-        <v>120</v>
+        <v>2284</v>
       </c>
       <c r="H192" s="177">
         <v>43</v>
@@ -60677,7 +61556,7 @@
       <c r="U224" s="210"/>
       <c r="V224" s="210"/>
     </row>
-    <row r="225" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="225" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A225" s="199" t="s">
         <v>1765</v>
       </c>
@@ -60723,7 +61602,7 @@
       <c r="U225" s="210"/>
       <c r="V225" s="210"/>
     </row>
-    <row r="226" spans="1:26" ht="15" customHeight="1">
+    <row r="226" spans="1:28" ht="15" customHeight="1">
       <c r="A226" s="177" t="s">
         <v>1770</v>
       </c>
@@ -60790,7 +61669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="227" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="227" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A227" s="177" t="s">
         <v>1777</v>
       </c>
@@ -60850,7 +61729,7 @@
         <v>2865</v>
       </c>
     </row>
-    <row r="228" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="228" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A228" s="177" t="s">
         <v>1779</v>
       </c>
@@ -60908,7 +61787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="229" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A229" s="199" t="s">
         <v>1782</v>
       </c>
@@ -60969,7 +61848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="230" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A230" s="199" t="s">
         <v>1875</v>
       </c>
@@ -61017,7 +61896,7 @@
       <c r="U230" s="210"/>
       <c r="V230" s="212"/>
     </row>
-    <row r="231" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="231" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A231" s="199" t="s">
         <v>1956</v>
       </c>
@@ -61063,7 +61942,7 @@
       <c r="U231" s="210"/>
       <c r="V231" s="210"/>
     </row>
-    <row r="232" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="232" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A232" s="199" t="s">
         <v>1958</v>
       </c>
@@ -61101,7 +61980,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="233" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="233" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A233" s="199" t="s">
         <v>1961</v>
       </c>
@@ -61139,7 +62018,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="234" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="234" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A234" s="197" t="s">
         <v>2194</v>
       </c>
@@ -61179,7 +62058,7 @@
         <v>97.012365091844799</v>
       </c>
     </row>
-    <row r="235" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="235" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A235" s="234" t="s">
         <v>2605</v>
       </c>
@@ -61224,7 +62103,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="236" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="236" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A236" s="221" t="s">
         <v>2884</v>
       </c>
@@ -61266,7 +62145,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="237" spans="1:26" ht="15" customHeight="1">
+    <row r="237" spans="1:28" ht="15" customHeight="1">
       <c r="A237" s="221" t="s">
         <v>2885</v>
       </c>
@@ -61311,7 +62190,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="238" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="238" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A238" s="221" t="s">
         <v>2879</v>
       </c>
@@ -61347,7 +62226,7 @@
         <v>2861</v>
       </c>
     </row>
-    <row r="239" spans="1:26" ht="15" hidden="1" customHeight="1">
+    <row r="239" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A239" s="221" t="s">
         <v>2880</v>
       </c>
@@ -61389,7 +62268,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="240" spans="1:26" ht="15" customHeight="1">
+    <row r="240" spans="1:28" ht="15" customHeight="1">
       <c r="A240" s="221" t="s">
         <v>2886</v>
       </c>
@@ -61437,6 +62316,9 @@
       </c>
       <c r="Z240">
         <v>2</v>
+      </c>
+      <c r="AB240">
+        <v>1</v>
       </c>
     </row>
     <row r="241" spans="1:27" ht="15" hidden="1" customHeight="1">
@@ -62087,7 +62969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:27" ht="15" customHeight="1">
+    <row r="257" spans="1:28" ht="15" customHeight="1">
       <c r="A257" s="221" t="s">
         <v>2870</v>
       </c>
@@ -62134,7 +63016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="258" spans="1:27" ht="15" customHeight="1">
+    <row r="258" spans="1:28" ht="15" customHeight="1">
       <c r="A258" s="221" t="s">
         <v>2881</v>
       </c>
@@ -62181,7 +63063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="259" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="259" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A259" s="223" t="s">
         <v>2892</v>
       </c>
@@ -62217,7 +63099,7 @@
         <v>2861</v>
       </c>
     </row>
-    <row r="260" spans="1:27" ht="15" customHeight="1">
+    <row r="260" spans="1:28" ht="15" customHeight="1">
       <c r="A260" s="221" t="s">
         <v>2893</v>
       </c>
@@ -62261,8 +63143,11 @@
       <c r="Z260">
         <v>2</v>
       </c>
-    </row>
-    <row r="261" spans="1:27" ht="15" hidden="1" customHeight="1">
+      <c r="AB260">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A261" s="221" t="s">
         <v>2894</v>
       </c>
@@ -62300,7 +63185,7 @@
         <v>2861</v>
       </c>
     </row>
-    <row r="262" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="262" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A262" s="221" t="s">
         <v>2895</v>
       </c>
@@ -62336,7 +63221,7 @@
         <v>2861</v>
       </c>
     </row>
-    <row r="263" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="263" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A263" s="221" t="s">
         <v>2896</v>
       </c>
@@ -62370,7 +63255,7 @@
         <v>2861</v>
       </c>
     </row>
-    <row r="264" spans="1:27" ht="15" customHeight="1">
+    <row r="264" spans="1:28" ht="15" customHeight="1">
       <c r="A264" s="221" t="s">
         <v>2874</v>
       </c>
@@ -62412,8 +63297,11 @@
       <c r="Z264">
         <v>2</v>
       </c>
-    </row>
-    <row r="265" spans="1:27" ht="15" customHeight="1">
+      <c r="AB264">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="265" spans="1:28" ht="15" customHeight="1">
       <c r="A265" s="221" t="s">
         <v>2875</v>
       </c>
@@ -62454,8 +63342,11 @@
       <c r="Z265">
         <v>2</v>
       </c>
-    </row>
-    <row r="266" spans="1:27" ht="15" customHeight="1">
+      <c r="AB265">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266" spans="1:28" ht="15" customHeight="1">
       <c r="A266" s="221" t="s">
         <v>2906</v>
       </c>
@@ -62497,7 +63388,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="267" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="267" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A267" s="221" t="s">
         <v>2873</v>
       </c>
@@ -62543,7 +63434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="268" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A268" s="221" t="s">
         <v>2877</v>
       </c>
@@ -62589,7 +63480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:27" ht="15" customHeight="1">
+    <row r="269" spans="1:28" ht="15" customHeight="1">
       <c r="A269" s="221" t="s">
         <v>2876</v>
       </c>
@@ -62633,8 +63524,11 @@
       <c r="Z269">
         <v>2</v>
       </c>
-    </row>
-    <row r="270" spans="1:27" ht="15" customHeight="1">
+      <c r="AB269">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="270" spans="1:28" ht="15" customHeight="1">
       <c r="A270" s="221" t="s">
         <v>2819</v>
       </c>
@@ -62682,7 +63576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:27" ht="15" hidden="1" customHeight="1">
+    <row r="271" spans="1:28" ht="15" hidden="1" customHeight="1">
       <c r="A271" s="221" t="s">
         <v>2985</v>
       </c>
@@ -62710,7 +63604,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="272" spans="1:27" ht="15" customHeight="1">
+    <row r="272" spans="1:28" ht="15" customHeight="1">
       <c r="A272" s="221" t="s">
         <v>3104</v>
       </c>
@@ -63218,10 +64112,25 @@
       </c>
     </row>
     <row r="290" spans="1:26" ht="15" customHeight="1">
+      <c r="A290" s="269" t="s">
+        <v>3168</v>
+      </c>
+      <c r="G290" s="270" t="s">
+        <v>120</v>
+      </c>
+      <c r="H290">
+        <v>43</v>
+      </c>
+      <c r="I290" s="272">
+        <v>290</v>
+      </c>
+      <c r="L290" s="271" t="s">
+        <v>3169</v>
+      </c>
       <c r="V290" s="212"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AA289" xr:uid="{B522DC56-3FF5-3344-845C-95A0430599ED}">
+  <autoFilter ref="A1:AA290" xr:uid="{B522DC56-3FF5-3344-845C-95A0430599ED}">
     <filterColumn colId="6">
       <filters>
         <filter val="yes"/>
@@ -63231,218 +64140,218 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y273">
     <sortCondition ref="I2:I273"/>
   </sortState>
-  <conditionalFormatting sqref="E86:E89 E30:E36 E58:E67 E69:E79 E84 E91:E93 E81:E82 F29:H84 E95:E99 E101:E103 F86:H104 E130:E141 F115:H158 I6:I272 F2:F270 J3:K271 K273:K276 I277:I289 E6:H28 E3:I5 E38 E41:E56 E105:H113 E115:E118 E120:E121 E123:E126 E143:E144 E146 E148 E152 E154 E156:E158 D2:D3 D11:D37 D39:E40 D42:D83 D85:D111 D113:D114 D116:D119 D121:D122 D124:D143 D145:E145 D147:E147 D149:E151 D153:E153 D155:E155 D157:D160">
-    <cfRule type="containsText" dxfId="52" priority="63" operator="containsText" text="Yes">
+  <conditionalFormatting sqref="E86:E89 E30:E36 E58:E67 E69:E79 E84 E91:E93 E81:E82 F29:H84 E95:E99 E101:E103 F86:H104 E130:E141 F115:H158 I6:I272 F2:F270 J3:K271 K273:K276 E6:H28 E3:I5 E38 E41:E56 E105:H113 E115:E118 E120:E121 E123:E126 E143:E144 E146 E148 E152 E154 E156:E158 D2:D3 D11:D37 D39:E40 D42:D83 D85:D111 D113:D114 D116:D119 D121:D122 D124:D143 D145:E145 D147:E147 D149:E151 D153:E153 D155:E155 D157:D160 I277:I290">
+    <cfRule type="containsText" dxfId="103" priority="65" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(D2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E85">
-    <cfRule type="containsText" dxfId="51" priority="62" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="102" priority="64" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(E85))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G114:H114">
-    <cfRule type="containsText" dxfId="50" priority="57" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="101" priority="59" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G114))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G161:H161">
-    <cfRule type="containsText" dxfId="49" priority="56" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="100" priority="58" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G161))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G162:H162">
-    <cfRule type="containsText" dxfId="48" priority="55" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="99" priority="57" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G162))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G163:H163">
-    <cfRule type="containsText" dxfId="47" priority="54" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="98" priority="56" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G163))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G193:H193">
-    <cfRule type="containsText" dxfId="46" priority="53" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="97" priority="55" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G193))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G203:H203">
-    <cfRule type="containsText" dxfId="45" priority="52" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="96" priority="54" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G203))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G204:H204">
-    <cfRule type="containsText" dxfId="44" priority="51" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="95" priority="53" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G204))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G213:H213">
-    <cfRule type="containsText" dxfId="43" priority="50" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="94" priority="52" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G213))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G216:H216">
-    <cfRule type="containsText" dxfId="42" priority="49" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="93" priority="51" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G216))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G218:H218">
-    <cfRule type="containsText" dxfId="41" priority="48" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="92" priority="50" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G218))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G227:H227">
-    <cfRule type="containsText" dxfId="40" priority="47" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="91" priority="49" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G227))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G230:H230">
-    <cfRule type="containsText" dxfId="39" priority="46" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="90" priority="48" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G230))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G238:H238">
-    <cfRule type="containsText" dxfId="38" priority="45" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="89" priority="47" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G238))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G241:H241">
-    <cfRule type="containsText" dxfId="37" priority="44" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="88" priority="46" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G241))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G245:H245">
-    <cfRule type="containsText" dxfId="36" priority="43" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="87" priority="45" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G245))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G236:H236">
-    <cfRule type="containsText" dxfId="35" priority="42" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="86" priority="44" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G236))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G248:H248">
-    <cfRule type="containsText" dxfId="34" priority="41" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="85" priority="43" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G248))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G249:H249">
-    <cfRule type="containsText" dxfId="33" priority="40" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="84" priority="42" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G249))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H254">
-    <cfRule type="containsText" dxfId="32" priority="39" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="83" priority="41" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(H254))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G256:H256">
-    <cfRule type="containsText" dxfId="31" priority="38" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="82" priority="40" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G256))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G257:H257">
-    <cfRule type="containsText" dxfId="30" priority="37" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="81" priority="39" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G257))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G258:H258">
-    <cfRule type="containsText" dxfId="29" priority="36" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="80" priority="38" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G258))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G259:H259">
-    <cfRule type="containsText" dxfId="28" priority="35" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="79" priority="37" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G259))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G261:H261">
-    <cfRule type="containsText" dxfId="27" priority="34" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="78" priority="36" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G261))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G265:H265">
-    <cfRule type="containsText" dxfId="26" priority="33" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="77" priority="35" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G265))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G266:H266">
-    <cfRule type="containsText" dxfId="25" priority="32" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="76" priority="34" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G266))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G268:H268">
-    <cfRule type="containsText" dxfId="24" priority="31" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="75" priority="33" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G268))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G267:H267">
-    <cfRule type="containsText" dxfId="23" priority="30" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="74" priority="32" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G267))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G269:H269">
-    <cfRule type="containsText" dxfId="22" priority="29" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="73" priority="31" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G269))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G270:H271 H277:H289">
-    <cfRule type="containsText" dxfId="21" priority="28" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="72" priority="30" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G270))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J83:K108">
-    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="71" priority="26" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(J83))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J109:K158">
-    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="70" priority="25" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(J109))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L82">
-    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="69" priority="24" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(L3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L83:L108">
-    <cfRule type="containsText" dxfId="17" priority="21" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="68" priority="23" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(L83))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L109:L158">
-    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="67" priority="22" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(L109))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:M82">
-    <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="66" priority="21" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M83:M108">
-    <cfRule type="containsText" dxfId="14" priority="18" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="65" priority="20" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M83))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M109:M158">
-    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="64" priority="19" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M109))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1">
-    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="63" priority="16" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(I1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:H1">
-    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="62" priority="15" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1">
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -63454,42 +64363,42 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F82:F107">
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="61" priority="12" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(F82))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F108:F157">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="60" priority="11" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(F108))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G254">
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="59" priority="10" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G254))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G255">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="58" priority="9" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G255))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G260">
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="57" priority="8" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G260))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G264">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="56" priority="7" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G264))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G272">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="55" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G272))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3:R271">
-    <cfRule type="colorScale" priority="69">
+    <cfRule type="colorScale" priority="71">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -63501,7 +64410,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R272">
-    <cfRule type="colorScale" priority="70">
+    <cfRule type="colorScale" priority="72">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -63513,18 +64422,30 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G277:G289">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="54" priority="5" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(G277))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F277:F289">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="53" priority="4" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(F277))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D277:D289 D242:D272 D239:D240 D237 D235 D226:D228 D202:D203">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="52" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(D202))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R1:R1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
@@ -63548,8 +64469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F0DA957-6899-A948-BF9C-0A6CA3970A65}">
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -64638,7 +65559,7 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="G2:G25 G33:G36">
-    <cfRule type="containsBlanks" dxfId="0" priority="54">
+    <cfRule type="containsBlanks" dxfId="156" priority="54">
       <formula>LEN(TRIM(#REF!))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>